<commit_message>
modificación base de datos
</commit_message>
<xml_diff>
--- a/datosProyecto.xlsx
+++ b/datosProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAROLD\Documents\proyectoFinalTeoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13449A2A-C18B-4B76-8003-EE55A1F0FB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3E96A6-CC9A-4B04-8835-F3C888C3AC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB8B80A4-B1C2-43E9-AEBE-A99F583F1180}"/>
   </bookViews>
@@ -892,7 +892,7 @@
   <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -982,10 +982,10 @@
         <v>18</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s">
         <v>21</v>
@@ -1029,7 +1029,7 @@
         <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N3" t="s">
         <v>26</v>
@@ -1076,10 +1076,10 @@
         <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s">
         <v>32</v>
@@ -1123,7 +1123,7 @@
         <v>35</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
         <v>26</v>
@@ -1173,7 +1173,7 @@
         <v>38</v>
       </c>
       <c r="N6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s">
         <v>36</v>
@@ -1217,7 +1217,7 @@
         <v>18</v>
       </c>
       <c r="M7" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N7" t="s">
         <v>26</v>
@@ -1264,10 +1264,10 @@
         <v>18</v>
       </c>
       <c r="M8" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="N8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O8" t="s">
         <v>42</v>
@@ -1311,10 +1311,10 @@
         <v>30</v>
       </c>
       <c r="M9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O9" t="s">
         <v>36</v>
@@ -1358,7 +1358,7 @@
         <v>18</v>
       </c>
       <c r="M10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N10" t="s">
         <v>31</v>
@@ -1405,7 +1405,7 @@
         <v>18</v>
       </c>
       <c r="M11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="N11" t="s">
         <v>26</v>
@@ -1452,10 +1452,10 @@
         <v>18</v>
       </c>
       <c r="M12" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O12" t="s">
         <v>36</v>
@@ -1499,10 +1499,10 @@
         <v>30</v>
       </c>
       <c r="M13" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="N13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O13" t="s">
         <v>21</v>
@@ -1546,7 +1546,7 @@
         <v>30</v>
       </c>
       <c r="M14" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="N14" t="s">
         <v>26</v>
@@ -1593,10 +1593,10 @@
         <v>24</v>
       </c>
       <c r="M15" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O15" t="s">
         <v>36</v>
@@ -1640,7 +1640,7 @@
         <v>18</v>
       </c>
       <c r="M16" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
         <v>26</v>
@@ -1687,10 +1687,10 @@
         <v>18</v>
       </c>
       <c r="M17" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="N17" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O17" t="s">
         <v>32</v>
@@ -1737,7 +1737,7 @@
         <v>25</v>
       </c>
       <c r="N18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O18" t="s">
         <v>32</v>
@@ -1781,10 +1781,10 @@
         <v>18</v>
       </c>
       <c r="M19" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N19" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O19" t="s">
         <v>36</v>
@@ -1828,10 +1828,10 @@
         <v>24</v>
       </c>
       <c r="M20" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O20" t="s">
         <v>36</v>
@@ -1875,10 +1875,10 @@
         <v>18</v>
       </c>
       <c r="M21" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N21" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O21" t="s">
         <v>32</v>
@@ -1925,7 +1925,7 @@
         <v>19</v>
       </c>
       <c r="N22" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="O22" t="s">
         <v>27</v>
@@ -1969,7 +1969,7 @@
         <v>18</v>
       </c>
       <c r="M23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N23" t="s">
         <v>26</v>
@@ -2016,10 +2016,10 @@
         <v>18</v>
       </c>
       <c r="M24" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O24" t="s">
         <v>36</v>
@@ -2063,7 +2063,7 @@
         <v>18</v>
       </c>
       <c r="M25" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N25" t="s">
         <v>26</v>
@@ -2113,7 +2113,7 @@
         <v>25</v>
       </c>
       <c r="N26" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O26" t="s">
         <v>32</v>
@@ -2157,10 +2157,10 @@
         <v>18</v>
       </c>
       <c r="M27" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="N27" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O27" t="s">
         <v>36</v>
@@ -2204,7 +2204,7 @@
         <v>35</v>
       </c>
       <c r="M28" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N28" t="s">
         <v>31</v>
@@ -2251,10 +2251,10 @@
         <v>24</v>
       </c>
       <c r="M29" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="N29" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O29" t="s">
         <v>32</v>
@@ -2298,10 +2298,10 @@
         <v>18</v>
       </c>
       <c r="M30" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N30" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O30" t="s">
         <v>36</v>
@@ -2345,10 +2345,10 @@
         <v>24</v>
       </c>
       <c r="M31" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N31" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O31" t="s">
         <v>27</v>
@@ -2392,10 +2392,10 @@
         <v>18</v>
       </c>
       <c r="M32" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N32" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O32" t="s">
         <v>36</v>
@@ -2439,10 +2439,10 @@
         <v>18</v>
       </c>
       <c r="M33" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="N33" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O33" t="s">
         <v>32</v>
@@ -2486,7 +2486,7 @@
         <v>18</v>
       </c>
       <c r="M34" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N34" t="s">
         <v>20</v>
@@ -2533,7 +2533,7 @@
         <v>18</v>
       </c>
       <c r="M35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N35" t="s">
         <v>26</v>
@@ -2583,7 +2583,7 @@
         <v>38</v>
       </c>
       <c r="N36" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O36" t="s">
         <v>21</v>
@@ -2627,7 +2627,7 @@
         <v>18</v>
       </c>
       <c r="M37" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N37" t="s">
         <v>26</v>
@@ -2674,10 +2674,10 @@
         <v>24</v>
       </c>
       <c r="M38" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="N38" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O38" t="s">
         <v>36</v>
@@ -2721,10 +2721,10 @@
         <v>24</v>
       </c>
       <c r="M39" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N39" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O39" t="s">
         <v>27</v>
@@ -2771,7 +2771,7 @@
         <v>19</v>
       </c>
       <c r="N40" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O40" t="s">
         <v>36</v>
@@ -2815,10 +2815,10 @@
         <v>18</v>
       </c>
       <c r="M41" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="N41" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O41" t="s">
         <v>36</v>
@@ -2912,7 +2912,7 @@
         <v>38</v>
       </c>
       <c r="N43" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O43" t="s">
         <v>32</v>
@@ -2956,7 +2956,7 @@
         <v>18</v>
       </c>
       <c r="M44" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N44" t="s">
         <v>31</v>
@@ -3003,10 +3003,10 @@
         <v>24</v>
       </c>
       <c r="M45" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="N45" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O45" t="s">
         <v>27</v>
@@ -3097,10 +3097,10 @@
         <v>24</v>
       </c>
       <c r="M47" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N47" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O47" t="s">
         <v>36</v>
@@ -3144,10 +3144,10 @@
         <v>35</v>
       </c>
       <c r="M48" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="N48" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O48" t="s">
         <v>27</v>
@@ -3194,7 +3194,7 @@
         <v>38</v>
       </c>
       <c r="N49" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O49" t="s">
         <v>36</v>
@@ -3285,10 +3285,10 @@
         <v>24</v>
       </c>
       <c r="M51" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N51" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O51" t="s">
         <v>32</v>
@@ -3332,7 +3332,7 @@
         <v>18</v>
       </c>
       <c r="M52" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N52" t="s">
         <v>31</v>
@@ -3379,10 +3379,10 @@
         <v>30</v>
       </c>
       <c r="M53" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="N53" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O53" t="s">
         <v>27</v>
@@ -3426,10 +3426,10 @@
         <v>30</v>
       </c>
       <c r="M54" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="N54" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O54" t="s">
         <v>32</v>
@@ -3520,10 +3520,10 @@
         <v>18</v>
       </c>
       <c r="M56" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="N56" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O56" t="s">
         <v>36</v>
@@ -3570,7 +3570,7 @@
         <v>25</v>
       </c>
       <c r="N57" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O57" t="s">
         <v>36</v>
@@ -3614,7 +3614,7 @@
         <v>18</v>
       </c>
       <c r="M58" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N58" t="s">
         <v>26</v>
@@ -3661,10 +3661,10 @@
         <v>24</v>
       </c>
       <c r="M59" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="N59" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O59" t="s">
         <v>27</v>
@@ -3708,10 +3708,10 @@
         <v>24</v>
       </c>
       <c r="M60" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N60" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O60" t="s">
         <v>27</v>
@@ -3755,10 +3755,10 @@
         <v>18</v>
       </c>
       <c r="M61" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N61" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O61" t="s">
         <v>32</v>
@@ -3802,7 +3802,7 @@
         <v>18</v>
       </c>
       <c r="M62" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N62" t="s">
         <v>26</v>
@@ -3852,7 +3852,7 @@
         <v>38</v>
       </c>
       <c r="N63" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O63" t="s">
         <v>32</v>
@@ -3896,7 +3896,7 @@
         <v>24</v>
       </c>
       <c r="M64" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N64" t="s">
         <v>26</v>
@@ -3943,7 +3943,7 @@
         <v>35</v>
       </c>
       <c r="M65" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N65" t="s">
         <v>26</v>
@@ -4037,10 +4037,10 @@
         <v>24</v>
       </c>
       <c r="M67" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N67" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O67" t="s">
         <v>21</v>
@@ -4084,10 +4084,10 @@
         <v>24</v>
       </c>
       <c r="M68" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N68" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O68" t="s">
         <v>36</v>
@@ -4131,7 +4131,7 @@
         <v>24</v>
       </c>
       <c r="M69" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N69" t="s">
         <v>26</v>
@@ -4181,7 +4181,7 @@
         <v>38</v>
       </c>
       <c r="N70" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O70" t="s">
         <v>36</v>
@@ -4225,10 +4225,10 @@
         <v>18</v>
       </c>
       <c r="M71" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="N71" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O71" t="s">
         <v>36</v>
@@ -4272,10 +4272,10 @@
         <v>18</v>
       </c>
       <c r="M72" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N72" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O72" t="s">
         <v>36</v>
@@ -4319,7 +4319,7 @@
         <v>24</v>
       </c>
       <c r="M73" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N73" t="s">
         <v>31</v>
@@ -4369,7 +4369,7 @@
         <v>38</v>
       </c>
       <c r="N74" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O74" t="s">
         <v>36</v>
@@ -4413,10 +4413,10 @@
         <v>30</v>
       </c>
       <c r="M75" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N75" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O75" t="s">
         <v>27</v>
@@ -4460,10 +4460,10 @@
         <v>18</v>
       </c>
       <c r="M76" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N76" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="O76" t="s">
         <v>32</v>
@@ -4507,10 +4507,10 @@
         <v>35</v>
       </c>
       <c r="M77" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N77" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O77" t="s">
         <v>36</v>
@@ -4554,7 +4554,7 @@
         <v>24</v>
       </c>
       <c r="M78" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N78" t="s">
         <v>31</v>
@@ -4601,10 +4601,10 @@
         <v>30</v>
       </c>
       <c r="M79" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="N79" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O79" t="s">
         <v>32</v>
@@ -4648,7 +4648,7 @@
         <v>24</v>
       </c>
       <c r="M80" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="N80" t="s">
         <v>26</v>
@@ -4695,10 +4695,10 @@
         <v>18</v>
       </c>
       <c r="M81" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="N81" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O81" t="s">
         <v>27</v>
@@ -4836,7 +4836,7 @@
         <v>18</v>
       </c>
       <c r="M84" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N84" t="s">
         <v>31</v>
@@ -4933,7 +4933,7 @@
         <v>38</v>
       </c>
       <c r="N86" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O86" t="s">
         <v>36</v>
@@ -4977,7 +4977,7 @@
         <v>24</v>
       </c>
       <c r="M87" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N87" t="s">
         <v>31</v>
@@ -5071,7 +5071,7 @@
         <v>24</v>
       </c>
       <c r="M89" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N89" t="s">
         <v>26</v>
@@ -5118,10 +5118,10 @@
         <v>24</v>
       </c>
       <c r="M90" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N90" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O90" t="s">
         <v>36</v>
@@ -5212,7 +5212,7 @@
         <v>18</v>
       </c>
       <c r="M92" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="N92" t="s">
         <v>31</v>
@@ -5306,7 +5306,7 @@
         <v>18</v>
       </c>
       <c r="M94" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="N94" t="s">
         <v>26</v>
@@ -5356,7 +5356,7 @@
         <v>38</v>
       </c>
       <c r="N95" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O95" t="s">
         <v>36</v>
@@ -5403,7 +5403,7 @@
         <v>38</v>
       </c>
       <c r="N96" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O96" t="s">
         <v>27</v>
@@ -5494,7 +5494,7 @@
         <v>35</v>
       </c>
       <c r="M98" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N98" t="s">
         <v>20</v>
@@ -5541,7 +5541,7 @@
         <v>35</v>
       </c>
       <c r="M99" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N99" t="s">
         <v>26</v>
@@ -5591,7 +5591,7 @@
         <v>38</v>
       </c>
       <c r="N100" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O100" t="s">
         <v>36</v>

</xml_diff>